<commit_message>
update Test cases file
</commit_message>
<xml_diff>
--- a/docs/Test Cases.xlsx
+++ b/docs/Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="125">
   <si>
     <t>Test case</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>Unit field can input number, it's not reasonable.</t>
-  </si>
-  <si>
-    <t>If the name saved twice, the page will show "DATABASE ERROR".</t>
   </si>
   <si>
     <t>List of Medicines</t>
@@ -495,6 +492,69 @@
         <family val="2"/>
       </rPr>
       <t>es</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>es</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The user should never see the error of database. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">If the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">medicines with same </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">name saved twice, the page will show </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Medicine name duplicate" instead of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>"DATABASE ERROR".</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -870,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -918,7 +978,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -938,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -958,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -978,10 +1038,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1301,16 +1361,16 @@
         <v>13</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
@@ -1321,16 +1381,16 @@
         <v>13</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
@@ -1409,13 +1469,13 @@
         <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
         <v>24</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -1432,10 +1492,10 @@
         <v>24</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
@@ -1557,21 +1617,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
-      <c r="C39" t="s">
-        <v>73</v>
+      <c r="C39" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="D39" t="s">
         <v>69</v>
       </c>
-      <c r="F39" t="s">
-        <v>16</v>
+      <c r="E39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -1579,13 +1642,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
         <v>74</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>75</v>
-      </c>
-      <c r="D40" t="s">
-        <v>76</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
@@ -1596,13 +1659,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
         <v>77</v>
       </c>
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F41" t="s">
         <v>9</v>
@@ -1613,13 +1676,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F42" t="s">
         <v>9</v>
@@ -1630,13 +1693,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
         <v>80</v>
       </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F43" t="s">
         <v>9</v>
@@ -1647,13 +1710,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
         <v>82</v>
       </c>
-      <c r="C44" t="s">
-        <v>83</v>
-      </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F44" t="s">
         <v>60</v>
@@ -1664,10 +1727,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
         <v>84</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
       </c>
       <c r="D45" t="s">
         <v>24</v>
@@ -1709,28 +1772,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>3</v>
@@ -1741,10 +1804,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="2">
         <v>51</v>
@@ -1756,10 +1819,10 @@
         <v>15.7</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>9</v>
@@ -1773,10 +1836,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D3" s="2">
         <v>52</v>
@@ -1788,10 +1851,10 @@
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
@@ -1805,10 +1868,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D4" s="2">
         <v>60</v>
@@ -1820,10 +1883,10 @@
         <v>18.5</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
@@ -1837,10 +1900,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D5" s="2">
         <v>82</v>
@@ -1852,10 +1915,10 @@
         <v>25.3</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>9</v>
@@ -1869,10 +1932,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -1884,10 +1947,10 @@
         <v>30.9</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>9</v>
@@ -1901,10 +1964,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D7" s="2">
         <v>130</v>
@@ -1916,10 +1979,10 @@
         <v>40.1</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>9</v>
@@ -1945,10 +2008,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2">
         <v>50</v>
@@ -1960,10 +2023,10 @@
         <v>13.9</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>9</v>
@@ -1977,10 +2040,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="2">
         <v>60</v>
@@ -1992,10 +2055,10 @@
         <v>16.600000000000001</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>9</v>
@@ -2009,10 +2072,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="2">
         <v>80</v>
@@ -2024,10 +2087,10 @@
         <v>22.2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>9</v>
@@ -2041,10 +2104,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="2">
         <v>90</v>
@@ -2056,10 +2119,10 @@
         <v>24.9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>
@@ -2073,10 +2136,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="2">
         <v>100</v>
@@ -2088,10 +2151,10 @@
         <v>27.7</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>9</v>
@@ -2105,10 +2168,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="2">
         <v>130</v>
@@ -2120,10 +2183,10 @@
         <v>36</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>9</v>
@@ -2167,31 +2230,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>3</v>
@@ -2202,10 +2265,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="2">
         <v>51</v>
@@ -2220,7 +2283,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I2" s="2">
         <v>51.8</v>
@@ -2237,10 +2300,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D3" s="2">
         <v>52</v>
@@ -2255,7 +2318,7 @@
         <v>18.5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" s="2">
         <v>59.9</v>
@@ -2272,10 +2335,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D4" s="2">
         <v>82</v>
@@ -2290,7 +2353,7 @@
         <v>24.9</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="2">
         <v>80.7</v>
@@ -2307,10 +2370,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
@@ -2325,7 +2388,7 @@
         <v>29.9</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" s="2">
         <v>96.9</v>
@@ -2342,10 +2405,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D6" s="2">
         <v>130</v>
@@ -2360,7 +2423,7 @@
         <v>39.9</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" s="2">
         <v>129.30000000000001</v>
@@ -2390,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
@@ -2408,7 +2471,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="2">
         <v>57.8</v>
@@ -2425,10 +2488,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2">
         <v>60</v>
@@ -2443,7 +2506,7 @@
         <v>18.5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I9" s="2">
         <v>66.8</v>
@@ -2460,10 +2523,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="2">
         <v>90</v>
@@ -2478,7 +2541,7 @@
         <v>22.9</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I10" s="2">
         <v>82.7</v>
@@ -2495,10 +2558,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="2">
         <v>100</v>
@@ -2513,7 +2576,7 @@
         <v>24.9</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I11" s="2">
         <v>89.9</v>
@@ -2530,10 +2593,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="2">
         <v>130</v>
@@ -2548,7 +2611,7 @@
         <v>34.9</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I12" s="2">
         <v>126</v>

</xml_diff>